<commit_message>
Updated about tab description
</commit_message>
<xml_diff>
--- a/Tax_Rate_Data_Analysis/tax_rate_data.xlsx
+++ b/Tax_Rate_Data_Analysis/tax_rate_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feng\OneDrive\Desktop\python\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feng\OneDrive\Desktop\Exploratory-Data-Analysis\Tax_Rate_Data_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B0ED145-9355-41CD-9BB4-E89F41060C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854E7710-AFFA-419F-8F5E-C66361EAFCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="2" r:id="rId1"/>
@@ -157,7 +157,7 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t>the tax_rate tab in this file includes Shopee's tax rates data for different types of fees for each month in 2022 for Southeast Asia countries. The tax_type column contains a complete list of tax types, and every country should have every tax type. The effective_month column stores the year-month info, where "beginning" refers to the first month of 2022</t>
+      <t>the tax_rate tab in this file includes company tax rates data for different types of fees for each month in 2022 for Southeast Asia countries. The tax_type column contains a complete list of tax types, and every country should have every tax type. The effective_month column stores the year-month info, where "beginning" refers to the first month of 2022</t>
     </r>
   </si>
 </sst>
@@ -1039,7 +1039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1061,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>